<commit_message>
Check table thru clev
</commit_message>
<xml_diff>
--- a/docs/fesity_check_table.xlsx
+++ b/docs/fesity_check_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cpetrik/Dropbox/Princeton/FEISTY/CODE/fish-offline/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AC82D5A-59B9-E940-9C08-6E2D026532AC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9EE8E14-9556-CB40-884B-F3F52EAFDA60}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1580" yWindow="460" windowWidth="15620" windowHeight="16560" xr2:uid="{75A10E79-64A5-084D-ADB9-F0FE4D64B0E0}"/>
+    <workbookView xWindow="1580" yWindow="460" windowWidth="15740" windowHeight="17540" xr2:uid="{75A10E79-64A5-084D-ADB9-F0FE4D64B0E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1037" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1751" uniqueCount="394">
   <si>
     <t>param = make_parameters_1meso()</t>
   </si>
@@ -1099,6 +1099,114 @@
   </si>
   <si>
     <t>Sf.con_zm = sub_cons(param,ENVR.Tp,ENVR.Tb,Sf.td,param.M_s,Sf.enc_zm)</t>
+  </si>
+  <si>
+    <t>param.kc</t>
+  </si>
+  <si>
+    <t>Sp.con_zm = sub_cons(param,ENVR.Tp,ENVR.Tb,Sp.td,param.M_s,Sp.enc_zm)</t>
+  </si>
+  <si>
+    <t>Sd.con_zm = sub_cons(param,ENVR.Tp,ENVR.Tb,Sd.td,param.M_s,Sd.enc_zm)</t>
+  </si>
+  <si>
+    <t>Mf.con_zm = sub_cons(param,ENVR.Tp,ENVR.Tb,Mf.td,param.M_m,[Mf.enc_zm,Mf.enc_f,Mf.enc_p,Mf.enc_d])</t>
+  </si>
+  <si>
+    <t>Mf.con_f  = sub_cons(param,ENVR.Tp,ENVR.Tb,Mf.td,param.M_m,[Mf.enc_f,Mf.enc_zm,Mf.enc_p,Mf.enc_d])</t>
+  </si>
+  <si>
+    <t>Mf.con_p  = sub_cons(param,ENVR.Tp,ENVR.Tb,Mf.td,param.M_m,[Mf.enc_p,Mf.enc_zm,Mf.enc_f,Mf.enc_d])</t>
+  </si>
+  <si>
+    <t>Mf.con_d  = sub_cons(param,ENVR.Tp,ENVR.Tb,Mf.td,param.M_m,[Mf.enc_d,Mf.enc_zm,Mf.enc_f,Mf.enc_p])</t>
+  </si>
+  <si>
+    <t>Mp.con_zm = sub_cons(param,ENVR.Tp,ENVR.Tb,Mp.td,param.M_m,[Mp.enc_zm,Mp.enc_f,Mp.enc_p,Mp.enc_d])</t>
+  </si>
+  <si>
+    <t>Mp.con_f  = sub_cons(param,ENVR.Tp,ENVR.Tb,Mp.td,param.M_m,[Mp.enc_f,Mp.enc_zm,Mp.enc_p,Mp.enc_d])</t>
+  </si>
+  <si>
+    <t>Mp.con_p  = sub_cons(param,ENVR.Tp,ENVR.Tb,Mp.td,param.M_m,[Mp.enc_p,Mp.enc_zm,Mp.enc_f,Mp.enc_d])</t>
+  </si>
+  <si>
+    <t>Mp.con_d  = sub_cons(param,ENVR.Tp,ENVR.Tb,Mp.td,param.M_m,[Mp.enc_d,Mp.enc_zm,Mp.enc_f,Mp.enc_p])</t>
+  </si>
+  <si>
+    <t>Md.con_be = sub_cons(param,ENVR.Tp,ENVR.Tb,Md.td,param.M_m,Md.enc_be)</t>
+  </si>
+  <si>
+    <t>Lp.con_f  = sub_cons(param,ENVR.Tp,ENVR.Tb,Lp.td,param.M_l,[Lp.enc_f,Lp.enc_p,Lp.enc_d])</t>
+  </si>
+  <si>
+    <t>Lp.con_p  = sub_cons(param,ENVR.Tp,ENVR.Tb,Lp.td,param.M_l,[Lp.enc_p,Lp.enc_f,Lp.enc_d])</t>
+  </si>
+  <si>
+    <t>Lp.con_d  = sub_cons(param,ENVR.Tp,ENVR.Tb,Lp.td,param.M_l,[Lp.enc_d,Lp.enc_p,Lp.enc_f])</t>
+  </si>
+  <si>
+    <t>Ld.con_f  = sub_cons(param,ENVR.Tp,ENVR.Tb,Ld.td,param.M_l,[Ld.enc_f,Ld.enc_p,Ld.enc_d,Ld.enc_be]</t>
+  </si>
+  <si>
+    <t>Ld.con_p  = sub_cons(param,ENVR.Tp,ENVR.Tb,Ld.td,param.M_l,[Ld.enc_p,Ld.enc_f,Ld.enc_d,Ld.enc_be])</t>
+  </si>
+  <si>
+    <t>Ld.con_d  = sub_cons(param,ENVR.Tp,ENVR.Tb,Ld.td,param.M_l,[Ld.enc_d,Ld.enc_p,Ld.enc_f,Ld.enc_be])</t>
+  </si>
+  <si>
+    <t>Ld.con_be = sub_cons(param,ENVR.Tp,ENVR.Tb,Ld.td,param.M_l,[Ld.enc_be,Ld.enc_f,Ld.enc_p,Ld.enc_d])</t>
+  </si>
+  <si>
+    <t>[Sf.con_zm,Sp.con_zm,Sd.con_zm,Mf.con_zm,Mp.con_zm,ENVR.fZm] = sub_offline_zm(Sf.con_zm,Sp.con_zm,Sd.con_zm,Mf.con_zm,Mp.con_zm,Sf.bio,Sp.bio,Sd.bio,Mf.bio,Mp.bio,ENVR.dZm)</t>
+  </si>
+  <si>
+    <t>Sf.I = Sf.con_zm</t>
+  </si>
+  <si>
+    <t>Mf.I = Mf.con_zm + Mf.con_f + Mf.con_p + Mf.con_d</t>
+  </si>
+  <si>
+    <t>Sp.I = S.con_zm</t>
+  </si>
+  <si>
+    <t>Sd.I = Sd.con_zm</t>
+  </si>
+  <si>
+    <t>Mp.I = Mp.con_zm + Mp.con_f + Mp.con_p + Mp.con_d</t>
+  </si>
+  <si>
+    <t>Md.I = Md.con_be</t>
+  </si>
+  <si>
+    <t>Lp.I = Lp.con_f + Lp.con_p + Lp.con_d</t>
+  </si>
+  <si>
+    <t>Ld.I = Ld.con_f + Ld.con_p + Ld.con_d + Ld.con_be</t>
+  </si>
+  <si>
+    <t>Sf.clev = sub_clev(param,Sf.I,ENVR.Tp,ENVR.Tb,Sf.td,param.M_s)</t>
+  </si>
+  <si>
+    <t>Sp.clev = sub_clev(param,Sp.I,ENVR.Tp,ENVR.Tb,Sp.td,param.M_s)</t>
+  </si>
+  <si>
+    <t>Sd.clev = sub_clev(param,Sd.I,ENVR.Tp,ENVR.Tb,Sd.td,param.M_s)</t>
+  </si>
+  <si>
+    <t>Mf.clev = sub_clev(param,Mf.I,ENVR.Tp,ENVR.Tb,Mf.td,param.M_m)</t>
+  </si>
+  <si>
+    <t>Mp.clev = sub_clev(param,Mp.I,ENVR.Tp,ENVR.Tb,Mp.td,param.M_m)</t>
+  </si>
+  <si>
+    <t>Md.clev = sub_clev(param,Md.I,ENVR.Tp,ENVR.Tb,Md.td,param.M_m)</t>
+  </si>
+  <si>
+    <t>Lp.clev = sub_clev(param,Lp.I,ENVR.Tp,ENVR.Tb,Lp.td,param.L_l)</t>
+  </si>
+  <si>
+    <t>Ld.clev = sub_clev(param,Ld.I,ENVR.Tp,ENVR.Tb,Ld.td,param.L_l)</t>
   </si>
 </sst>
 </file>
@@ -1482,10 +1590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05544419-54E0-4341-8244-0AE65D17B22B}">
-  <dimension ref="A3:G720"/>
+  <dimension ref="A3:G1148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A688" workbookViewId="0">
-      <selection activeCell="A719" sqref="A719"/>
+    <sheetView tabSelected="1" topLeftCell="A1115" workbookViewId="0">
+      <selection activeCell="A1140" sqref="A1140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9041,7 +9149,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="705" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="705" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B705" s="4" t="s">
         <v>1</v>
       </c>
@@ -9061,7 +9169,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="706" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="706" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B706" s="1" t="s">
         <v>32</v>
       </c>
@@ -9078,7 +9186,7 @@
         <v>1.44E-2</v>
       </c>
     </row>
-    <row r="707" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="707" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B707" s="1" t="s">
         <v>30</v>
       </c>
@@ -9086,7 +9194,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="708" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="708" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B708" s="1" t="s">
         <v>35</v>
       </c>
@@ -9094,7 +9202,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="709" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="709" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B709" s="1" t="s">
         <v>335</v>
       </c>
@@ -9102,7 +9210,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="710" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="710" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B710" t="s">
         <v>312</v>
       </c>
@@ -9113,7 +9221,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="711" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="711" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B711" t="s">
         <v>313</v>
       </c>
@@ -9124,7 +9232,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="712" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="712" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B712" s="1" t="s">
         <v>20</v>
       </c>
@@ -9132,7 +9240,7 @@
         <v>5590.2</v>
       </c>
     </row>
-    <row r="713" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="713" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B713" s="1" t="s">
         <v>324</v>
       </c>
@@ -9143,7 +9251,7 @@
         <v>0.72350000000000003</v>
       </c>
     </row>
-    <row r="714" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="714" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B714" s="1" t="s">
         <v>265</v>
       </c>
@@ -9154,7 +9262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="715" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="715" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B715" s="1" t="s">
         <v>355</v>
       </c>
@@ -9167,7 +9275,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="716" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="716" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B716" s="1" t="s">
         <v>56</v>
       </c>
@@ -9175,7 +9283,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="718" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="718" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C718" t="s">
         <v>81</v>
       </c>
@@ -9189,12 +9297,15 @@
         <v>82</v>
       </c>
     </row>
-    <row r="719" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="719" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A719" s="4">
+        <v>36</v>
+      </c>
       <c r="B719" s="3" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="720" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="720" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B720" s="4" t="s">
         <v>1</v>
       </c>
@@ -9212,6 +9323,4702 @@
       </c>
       <c r="G720" s="4" t="s">
         <v>80</v>
+      </c>
+    </row>
+    <row r="721" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B721" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="C721">
+        <v>6.3E-2</v>
+      </c>
+      <c r="E721" t="s">
+        <v>94</v>
+      </c>
+      <c r="F721">
+        <v>0.1139</v>
+      </c>
+      <c r="G721">
+        <v>0.18640000000000001</v>
+      </c>
+    </row>
+    <row r="722" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B722" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C722">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="723" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B723" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C723">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="724" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B724" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C724">
+        <v>9.6</v>
+      </c>
+      <c r="D724">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="725" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B725" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="C725">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="D725">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="726" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B726" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C726">
+        <v>1</v>
+      </c>
+      <c r="D726">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="727" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B727" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C727">
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="728" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B728" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C728">
+        <v>0.64790000000000003</v>
+      </c>
+      <c r="D728">
+        <v>1.8853</v>
+      </c>
+    </row>
+    <row r="730" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C730" t="s">
+        <v>81</v>
+      </c>
+      <c r="D730" t="s">
+        <v>82</v>
+      </c>
+      <c r="F730" t="s">
+        <v>81</v>
+      </c>
+      <c r="G730" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="731" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A731" s="4">
+        <v>37</v>
+      </c>
+      <c r="B731" s="3" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="732" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B732" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C732" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D732" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E732" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F732" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G732" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="733" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B733" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="C733">
+        <v>6.3E-2</v>
+      </c>
+      <c r="E733" t="s">
+        <v>120</v>
+      </c>
+      <c r="F733">
+        <v>0.1139</v>
+      </c>
+      <c r="G733">
+        <v>0.18640000000000001</v>
+      </c>
+    </row>
+    <row r="734" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B734" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C734">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="735" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B735" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C735">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="736" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B736" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C736">
+        <v>9.6</v>
+      </c>
+      <c r="D736">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="737" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B737" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="C737">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="D737">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="738" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B738" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="C738">
+        <v>1</v>
+      </c>
+      <c r="D738">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="739" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B739" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C739">
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="740" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B740" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C740">
+        <v>0.64790000000000003</v>
+      </c>
+      <c r="D740">
+        <v>1.8853</v>
+      </c>
+    </row>
+    <row r="742" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C742" t="s">
+        <v>81</v>
+      </c>
+      <c r="D742" t="s">
+        <v>82</v>
+      </c>
+      <c r="F742" t="s">
+        <v>81</v>
+      </c>
+      <c r="G742" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="743" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A743" s="4">
+        <v>38</v>
+      </c>
+      <c r="B743" s="3" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="744" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B744" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C744" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D744" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E744" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F744" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G744" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="745" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B745" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="C745">
+        <v>6.3E-2</v>
+      </c>
+      <c r="E745" t="s">
+        <v>146</v>
+      </c>
+      <c r="F745">
+        <v>0.1139</v>
+      </c>
+      <c r="G745">
+        <v>0.18640000000000001</v>
+      </c>
+    </row>
+    <row r="746" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B746" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C746">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="747" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B747" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C747">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="748" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B748" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C748">
+        <v>9.6</v>
+      </c>
+      <c r="D748">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="749" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B749" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="C749">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="D749">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="750" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B750" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C750">
+        <v>1</v>
+      </c>
+      <c r="D750">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="751" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B751" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C751">
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="752" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B752" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C752">
+        <v>0.64790000000000003</v>
+      </c>
+      <c r="D752">
+        <v>1.8853</v>
+      </c>
+    </row>
+    <row r="754" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C754" t="s">
+        <v>81</v>
+      </c>
+      <c r="D754" t="s">
+        <v>82</v>
+      </c>
+      <c r="F754" t="s">
+        <v>81</v>
+      </c>
+      <c r="G754" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="755" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A755" s="4">
+        <v>39</v>
+      </c>
+      <c r="B755" s="3" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="756" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B756" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C756" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D756" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E756" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F756" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G756" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="757" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B757" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="C757">
+        <v>6.3E-2</v>
+      </c>
+      <c r="E757" t="s">
+        <v>172</v>
+      </c>
+      <c r="F757">
+        <v>2.1700000000000001E-2</v>
+      </c>
+      <c r="G757">
+        <v>3.7100000000000001E-2</v>
+      </c>
+    </row>
+    <row r="758" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B758" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C758">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="759" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B759" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C759">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="760" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B760" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C760">
+        <v>9.6</v>
+      </c>
+      <c r="D760">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="761" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B761" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="C761">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="D761">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="762" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B762" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C762">
+        <v>1</v>
+      </c>
+      <c r="D762">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="763" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B763" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C763">
+        <v>11.180300000000001</v>
+      </c>
+    </row>
+    <row r="764" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B764" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C764">
+        <v>9.35E-2</v>
+      </c>
+      <c r="D764">
+        <v>0.27200000000000002</v>
+      </c>
+    </row>
+    <row r="765" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B765" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C765">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="D765">
+        <v>3.8E-3</v>
+      </c>
+    </row>
+    <row r="766" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B766" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C766" s="2">
+        <v>1.3850000000000001E-4</v>
+      </c>
+      <c r="D766" s="2">
+        <v>2.0719999999999999E-4</v>
+      </c>
+    </row>
+    <row r="767" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B767" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C767" s="2">
+        <v>5.5389999999999997E-4</v>
+      </c>
+      <c r="D767" s="2">
+        <v>8.2890000000000004E-4</v>
+      </c>
+    </row>
+    <row r="769" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C769" t="s">
+        <v>81</v>
+      </c>
+      <c r="D769" t="s">
+        <v>82</v>
+      </c>
+      <c r="F769" t="s">
+        <v>81</v>
+      </c>
+      <c r="G769" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="770" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A770" s="4">
+        <v>40</v>
+      </c>
+      <c r="B770" s="3" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="771" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B771" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C771" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D771" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E771" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F771" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G771" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="772" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B772" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="C772">
+        <v>6.3E-2</v>
+      </c>
+      <c r="E772" t="s">
+        <v>169</v>
+      </c>
+      <c r="F772" s="2">
+        <v>5.8909999999999995E-4</v>
+      </c>
+      <c r="G772" s="2">
+        <v>5.1829999999999997E-4</v>
+      </c>
+    </row>
+    <row r="773" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B773" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C773">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="774" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B774" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C774">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="775" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B775" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C775">
+        <v>9.6</v>
+      </c>
+      <c r="D775">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="776" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B776" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="C776">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="D776">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="777" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B777" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C777">
+        <v>1</v>
+      </c>
+      <c r="D777">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="778" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B778" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C778">
+        <v>11.180300000000001</v>
+      </c>
+    </row>
+    <row r="779" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B779" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C779">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="D779">
+        <v>3.8E-3</v>
+      </c>
+    </row>
+    <row r="780" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B780" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C780">
+        <v>9.35E-2</v>
+      </c>
+      <c r="D780">
+        <v>0.27200000000000002</v>
+      </c>
+    </row>
+    <row r="781" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B781" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C781" s="2">
+        <v>1.3850000000000001E-4</v>
+      </c>
+      <c r="D781" s="2">
+        <v>2.0719999999999999E-4</v>
+      </c>
+    </row>
+    <row r="782" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B782" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C782" s="2">
+        <v>5.5389999999999997E-4</v>
+      </c>
+      <c r="D782" s="2">
+        <v>8.2890000000000004E-4</v>
+      </c>
+    </row>
+    <row r="784" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C784" t="s">
+        <v>81</v>
+      </c>
+      <c r="D784" t="s">
+        <v>82</v>
+      </c>
+      <c r="F784" t="s">
+        <v>81</v>
+      </c>
+      <c r="G784" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="785" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A785" s="4">
+        <v>41</v>
+      </c>
+      <c r="B785" s="3" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="786" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B786" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C786" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D786" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E786" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F786" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G786" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="787" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B787" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="C787">
+        <v>6.3E-2</v>
+      </c>
+      <c r="E787" t="s">
+        <v>170</v>
+      </c>
+      <c r="F787" s="2">
+        <v>3.2129999999999999E-5</v>
+      </c>
+      <c r="G787" s="2">
+        <v>2.8269999999999999E-5</v>
+      </c>
+    </row>
+    <row r="788" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B788" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C788">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="789" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B789" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C789">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="790" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B790" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C790">
+        <v>9.6</v>
+      </c>
+      <c r="D790">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="791" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B791" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="C791">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="D791">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="792" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B792" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C792">
+        <v>1</v>
+      </c>
+      <c r="D792">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="793" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B793" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C793">
+        <v>11.180300000000001</v>
+      </c>
+    </row>
+    <row r="794" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B794" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C794" s="2">
+        <v>1.3850000000000001E-4</v>
+      </c>
+      <c r="D794" s="2">
+        <v>2.0719999999999999E-4</v>
+      </c>
+    </row>
+    <row r="795" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B795" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C795">
+        <v>9.35E-2</v>
+      </c>
+      <c r="D795">
+        <v>0.27200000000000002</v>
+      </c>
+    </row>
+    <row r="796" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B796" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C796">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="D796">
+        <v>3.8E-3</v>
+      </c>
+    </row>
+    <row r="797" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B797" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C797" s="2">
+        <v>5.5389999999999997E-4</v>
+      </c>
+      <c r="D797" s="2">
+        <v>8.2890000000000004E-4</v>
+      </c>
+    </row>
+    <row r="799" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C799" t="s">
+        <v>81</v>
+      </c>
+      <c r="D799" t="s">
+        <v>82</v>
+      </c>
+      <c r="F799" t="s">
+        <v>81</v>
+      </c>
+      <c r="G799" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="800" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A800" s="4">
+        <v>42</v>
+      </c>
+      <c r="B800" s="3" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="801" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B801" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C801" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D801" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E801" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F801" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G801" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="802" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B802" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="C802">
+        <v>6.3E-2</v>
+      </c>
+      <c r="E802" t="s">
+        <v>171</v>
+      </c>
+      <c r="F802" s="2">
+        <v>1.2850000000000001E-4</v>
+      </c>
+      <c r="G802" s="2">
+        <v>1.131E-4</v>
+      </c>
+    </row>
+    <row r="803" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B803" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C803">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="804" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B804" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C804">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="805" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B805" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C805">
+        <v>9.6</v>
+      </c>
+      <c r="D805">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="806" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B806" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="C806">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="D806">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="807" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B807" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C807">
+        <v>1</v>
+      </c>
+      <c r="D807">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="808" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B808" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C808">
+        <v>11.180300000000001</v>
+      </c>
+    </row>
+    <row r="809" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B809" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C809" s="2">
+        <v>5.5389999999999997E-4</v>
+      </c>
+      <c r="D809" s="2">
+        <v>8.2890000000000004E-4</v>
+      </c>
+    </row>
+    <row r="810" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B810" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C810">
+        <v>9.35E-2</v>
+      </c>
+      <c r="D810">
+        <v>0.27200000000000002</v>
+      </c>
+    </row>
+    <row r="811" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B811" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C811">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="D811">
+        <v>3.8E-3</v>
+      </c>
+    </row>
+    <row r="812" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B812" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C812" s="2">
+        <v>1.3850000000000001E-4</v>
+      </c>
+      <c r="D812" s="2">
+        <v>2.0719999999999999E-4</v>
+      </c>
+    </row>
+    <row r="814" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C814" t="s">
+        <v>81</v>
+      </c>
+      <c r="D814" t="s">
+        <v>82</v>
+      </c>
+      <c r="F814" t="s">
+        <v>81</v>
+      </c>
+      <c r="G814" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="815" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A815" s="4">
+        <v>43</v>
+      </c>
+      <c r="B815" s="3" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="816" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B816" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C816" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D816" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E816" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F816" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G816" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="817" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B817" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="C817">
+        <v>6.3E-2</v>
+      </c>
+      <c r="E817" t="s">
+        <v>198</v>
+      </c>
+      <c r="F817">
+        <v>2.1700000000000001E-2</v>
+      </c>
+      <c r="G817">
+        <v>3.7100000000000001E-2</v>
+      </c>
+    </row>
+    <row r="818" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B818" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C818">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="819" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B819" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C819">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="820" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B820" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C820">
+        <v>9.6</v>
+      </c>
+      <c r="D820">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="821" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B821" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="C821">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="D821">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="822" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B822" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C822">
+        <v>1</v>
+      </c>
+      <c r="D822">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="823" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B823" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C823">
+        <v>11.180300000000001</v>
+      </c>
+    </row>
+    <row r="824" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B824" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C824">
+        <v>9.35E-2</v>
+      </c>
+      <c r="D824">
+        <v>0.27200000000000002</v>
+      </c>
+    </row>
+    <row r="825" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B825" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C825">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="D825">
+        <v>3.8E-3</v>
+      </c>
+    </row>
+    <row r="826" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B826" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C826" s="2">
+        <v>1.3850000000000001E-4</v>
+      </c>
+      <c r="D826" s="2">
+        <v>2.0719999999999999E-4</v>
+      </c>
+    </row>
+    <row r="827" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B827" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C827" s="2">
+        <v>5.5389999999999997E-4</v>
+      </c>
+      <c r="D827" s="2">
+        <v>8.2890000000000004E-4</v>
+      </c>
+    </row>
+    <row r="829" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C829" t="s">
+        <v>81</v>
+      </c>
+      <c r="D829" t="s">
+        <v>82</v>
+      </c>
+      <c r="F829" t="s">
+        <v>81</v>
+      </c>
+      <c r="G829" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="830" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A830" s="4">
+        <v>44</v>
+      </c>
+      <c r="B830" s="3" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="831" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B831" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C831" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D831" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E831" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F831" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G831" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="832" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B832" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="C832">
+        <v>6.3E-2</v>
+      </c>
+      <c r="E832" t="s">
+        <v>195</v>
+      </c>
+      <c r="F832" s="2">
+        <v>5.8909999999999995E-4</v>
+      </c>
+      <c r="G832" s="2">
+        <v>5.1829999999999997E-4</v>
+      </c>
+    </row>
+    <row r="833" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B833" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C833">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="834" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B834" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C834">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="835" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B835" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C835">
+        <v>9.6</v>
+      </c>
+      <c r="D835">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="836" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B836" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="C836">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="D836">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="837" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B837" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C837">
+        <v>1</v>
+      </c>
+      <c r="D837">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="838" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B838" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C838">
+        <v>11.180300000000001</v>
+      </c>
+    </row>
+    <row r="839" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B839" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C839">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="D839">
+        <v>3.8E-3</v>
+      </c>
+    </row>
+    <row r="840" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B840" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C840">
+        <v>9.35E-2</v>
+      </c>
+      <c r="D840">
+        <v>0.27200000000000002</v>
+      </c>
+    </row>
+    <row r="841" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B841" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C841" s="2">
+        <v>1.3850000000000001E-4</v>
+      </c>
+      <c r="D841" s="2">
+        <v>2.0719999999999999E-4</v>
+      </c>
+    </row>
+    <row r="842" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B842" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C842" s="2">
+        <v>5.5389999999999997E-4</v>
+      </c>
+      <c r="D842" s="2">
+        <v>8.2890000000000004E-4</v>
+      </c>
+    </row>
+    <row r="844" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C844" t="s">
+        <v>81</v>
+      </c>
+      <c r="D844" t="s">
+        <v>82</v>
+      </c>
+      <c r="F844" t="s">
+        <v>81</v>
+      </c>
+      <c r="G844" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="845" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A845" s="4">
+        <v>45</v>
+      </c>
+      <c r="B845" s="3" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="846" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B846" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C846" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D846" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E846" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F846" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G846" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="847" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B847" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="C847">
+        <v>6.3E-2</v>
+      </c>
+      <c r="E847" t="s">
+        <v>196</v>
+      </c>
+      <c r="F847" s="2">
+        <v>3.2129999999999999E-5</v>
+      </c>
+      <c r="G847" s="2">
+        <v>2.8269999999999999E-5</v>
+      </c>
+    </row>
+    <row r="848" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B848" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C848">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="849" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B849" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C849">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="850" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B850" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C850">
+        <v>9.6</v>
+      </c>
+      <c r="D850">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="851" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B851" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="C851">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="D851">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="852" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B852" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C852">
+        <v>1</v>
+      </c>
+      <c r="D852">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="853" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B853" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C853">
+        <v>11.180300000000001</v>
+      </c>
+    </row>
+    <row r="854" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B854" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C854" s="2">
+        <v>1.3850000000000001E-4</v>
+      </c>
+      <c r="D854" s="2">
+        <v>2.0719999999999999E-4</v>
+      </c>
+    </row>
+    <row r="855" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B855" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C855">
+        <v>9.35E-2</v>
+      </c>
+      <c r="D855">
+        <v>0.27200000000000002</v>
+      </c>
+    </row>
+    <row r="856" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B856" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C856">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="D856">
+        <v>3.8E-3</v>
+      </c>
+    </row>
+    <row r="857" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B857" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C857" s="2">
+        <v>5.5389999999999997E-4</v>
+      </c>
+      <c r="D857" s="2">
+        <v>8.2890000000000004E-4</v>
+      </c>
+    </row>
+    <row r="859" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C859" t="s">
+        <v>81</v>
+      </c>
+      <c r="D859" t="s">
+        <v>82</v>
+      </c>
+      <c r="F859" t="s">
+        <v>81</v>
+      </c>
+      <c r="G859" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="860" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A860" s="4">
+        <v>46</v>
+      </c>
+      <c r="B860" s="3" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="861" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B861" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C861" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D861" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E861" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F861" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G861" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="862" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B862" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="C862">
+        <v>6.3E-2</v>
+      </c>
+      <c r="E862" t="s">
+        <v>197</v>
+      </c>
+      <c r="F862" s="2">
+        <v>1.2850000000000001E-4</v>
+      </c>
+      <c r="G862" s="2">
+        <v>1.131E-4</v>
+      </c>
+    </row>
+    <row r="863" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B863" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C863">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="864" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B864" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C864">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="865" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B865" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C865">
+        <v>9.6</v>
+      </c>
+      <c r="D865">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="866" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B866" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="C866">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="D866">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="867" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B867" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C867">
+        <v>1</v>
+      </c>
+      <c r="D867">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="868" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B868" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C868">
+        <v>11.180300000000001</v>
+      </c>
+    </row>
+    <row r="869" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B869" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C869" s="2">
+        <v>5.5389999999999997E-4</v>
+      </c>
+      <c r="D869" s="2">
+        <v>8.2890000000000004E-4</v>
+      </c>
+    </row>
+    <row r="870" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B870" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C870">
+        <v>9.35E-2</v>
+      </c>
+      <c r="D870">
+        <v>0.27200000000000002</v>
+      </c>
+    </row>
+    <row r="871" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B871" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C871">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="D871">
+        <v>3.8E-3</v>
+      </c>
+    </row>
+    <row r="872" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B872" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C872" s="2">
+        <v>1.3850000000000001E-4</v>
+      </c>
+      <c r="D872" s="2">
+        <v>2.0719999999999999E-4</v>
+      </c>
+    </row>
+    <row r="874" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C874" t="s">
+        <v>81</v>
+      </c>
+      <c r="D874" t="s">
+        <v>82</v>
+      </c>
+      <c r="F874" t="s">
+        <v>81</v>
+      </c>
+      <c r="G874" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="875" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A875" s="4">
+        <v>47</v>
+      </c>
+      <c r="B875" s="3" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="876" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B876" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C876" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D876" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E876" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F876" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G876" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="877" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B877" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="C877">
+        <v>6.3E-2</v>
+      </c>
+      <c r="E877" t="s">
+        <v>226</v>
+      </c>
+      <c r="F877">
+        <v>2.1399999999999999E-2</v>
+      </c>
+      <c r="G877" s="7">
+        <v>1.29E-2</v>
+      </c>
+    </row>
+    <row r="878" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B878" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C878">
+        <v>20</v>
+      </c>
+      <c r="G878" s="2"/>
+    </row>
+    <row r="879" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B879" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C879">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="880" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B880" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C880">
+        <v>9.6</v>
+      </c>
+      <c r="D880">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="881" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B881" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="C881">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="D881">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="882" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B882" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C882">
+        <v>0</v>
+      </c>
+      <c r="D882">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="883" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B883" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C883">
+        <v>11.180300000000001</v>
+      </c>
+    </row>
+    <row r="884" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B884" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C884" s="7">
+        <v>8.4599999999999995E-2</v>
+      </c>
+      <c r="D884">
+        <v>4.9799999999999997E-2</v>
+      </c>
+    </row>
+    <row r="886" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C886" t="s">
+        <v>81</v>
+      </c>
+      <c r="D886" t="s">
+        <v>82</v>
+      </c>
+      <c r="F886" t="s">
+        <v>81</v>
+      </c>
+      <c r="G886" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="887" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A887" s="4">
+        <v>48</v>
+      </c>
+      <c r="B887" s="3" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="888" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B888" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C888" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D888" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E888" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F888" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G888" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="889" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B889" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="C889">
+        <v>6.3E-2</v>
+      </c>
+      <c r="E889" t="s">
+        <v>247</v>
+      </c>
+      <c r="F889" s="2">
+        <v>4.8999999999999998E-3</v>
+      </c>
+      <c r="G889" s="2">
+        <v>7.4000000000000003E-3</v>
+      </c>
+    </row>
+    <row r="890" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B890" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C890">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="891" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B891" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C891">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="892" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B892" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C892">
+        <v>9.6</v>
+      </c>
+      <c r="D892">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="893" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B893" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="C893">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="D893">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="894" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B894" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C894">
+        <v>1</v>
+      </c>
+      <c r="D894">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="895" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B895" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C895" s="2">
+        <v>5590.2</v>
+      </c>
+    </row>
+    <row r="896" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B896" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C896" s="7">
+        <v>3.1600000000000003E-2</v>
+      </c>
+      <c r="D896">
+        <v>4.7300000000000002E-2</v>
+      </c>
+    </row>
+    <row r="897" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B897" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C897" s="2">
+        <v>1.9E-3</v>
+      </c>
+      <c r="D897" s="2">
+        <v>2.8E-3</v>
+      </c>
+    </row>
+    <row r="898" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B898" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C898" s="8">
+        <v>0</v>
+      </c>
+      <c r="D898" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="900" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C900" t="s">
+        <v>81</v>
+      </c>
+      <c r="D900" t="s">
+        <v>82</v>
+      </c>
+      <c r="F900" t="s">
+        <v>81</v>
+      </c>
+      <c r="G900" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="901" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A901" s="4">
+        <v>49</v>
+      </c>
+      <c r="B901" s="3" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="902" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B902" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C902" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D902" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E902" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F902" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G902" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="903" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B903" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="C903">
+        <v>6.3E-2</v>
+      </c>
+      <c r="E903" t="s">
+        <v>248</v>
+      </c>
+      <c r="F903" s="2">
+        <v>2.9530000000000002E-4</v>
+      </c>
+      <c r="G903" s="2">
+        <v>4.4200000000000001E-4</v>
+      </c>
+    </row>
+    <row r="904" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B904" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C904">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="905" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B905" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C905">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="906" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B906" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C906">
+        <v>9.6</v>
+      </c>
+      <c r="D906">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="907" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B907" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="C907">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="D907">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="908" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B908" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C908">
+        <v>1</v>
+      </c>
+      <c r="D908">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="909" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B909" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C909" s="2">
+        <v>5590.2</v>
+      </c>
+    </row>
+    <row r="910" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B910" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C910" s="2">
+        <v>1.9E-3</v>
+      </c>
+      <c r="D910" s="2">
+        <v>2.8E-3</v>
+      </c>
+    </row>
+    <row r="911" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B911" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C911" s="7">
+        <v>3.1600000000000003E-2</v>
+      </c>
+      <c r="D911">
+        <v>4.7300000000000002E-2</v>
+      </c>
+    </row>
+    <row r="912" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B912" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C912" s="8">
+        <v>0</v>
+      </c>
+      <c r="D912" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="914" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C914" t="s">
+        <v>81</v>
+      </c>
+      <c r="D914" t="s">
+        <v>82</v>
+      </c>
+      <c r="F914" t="s">
+        <v>81</v>
+      </c>
+      <c r="G914" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="915" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A915" s="4">
+        <v>50</v>
+      </c>
+      <c r="B915" s="3" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="916" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B916" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C916" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D916" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E916" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F916" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G916" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="917" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B917" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="C917">
+        <v>6.3E-2</v>
+      </c>
+      <c r="E917" t="s">
+        <v>249</v>
+      </c>
+      <c r="F917" s="8">
+        <v>0</v>
+      </c>
+      <c r="G917" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="918" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B918" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C918">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="919" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B919" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C919">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="920" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B920" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C920">
+        <v>9.6</v>
+      </c>
+      <c r="D920">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="921" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B921" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="C921">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="D921">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="922" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B922" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C922">
+        <v>1</v>
+      </c>
+      <c r="D922">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="923" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B923" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C923" s="2">
+        <v>5590.2</v>
+      </c>
+    </row>
+    <row r="924" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B924" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C924" s="8">
+        <v>0</v>
+      </c>
+      <c r="D924" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="925" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B925" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C925" s="7">
+        <v>3.1600000000000003E-2</v>
+      </c>
+      <c r="D925">
+        <v>4.7300000000000002E-2</v>
+      </c>
+    </row>
+    <row r="926" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B926" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C926" s="2">
+        <v>1.9E-3</v>
+      </c>
+      <c r="D926" s="2">
+        <v>2.8E-3</v>
+      </c>
+    </row>
+    <row r="928" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C928" t="s">
+        <v>81</v>
+      </c>
+      <c r="D928" t="s">
+        <v>82</v>
+      </c>
+      <c r="F928" t="s">
+        <v>81</v>
+      </c>
+      <c r="G928" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="929" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A929" s="4">
+        <v>51</v>
+      </c>
+      <c r="B929" s="3" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="930" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B930" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C930" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D930" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E930" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F930" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G930" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="931" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B931" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="C931">
+        <v>6.3E-2</v>
+      </c>
+      <c r="E931" t="s">
+        <v>273</v>
+      </c>
+      <c r="F931" s="2">
+        <v>2.3E-3</v>
+      </c>
+      <c r="G931" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="932" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B932" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C932">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="933" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B933" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C933">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="934" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B934" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C934">
+        <v>9.6</v>
+      </c>
+      <c r="D934">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="935" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B935" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="C935">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="D935">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="936" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B936" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="C936">
+        <v>0.4516</v>
+      </c>
+      <c r="D936">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="937" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B937" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C937" s="2">
+        <v>5590.2</v>
+      </c>
+    </row>
+    <row r="938" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B938" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="C938" s="7">
+        <v>2.35E-2</v>
+      </c>
+      <c r="D938" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="939" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B939" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C939">
+        <v>1.4E-3</v>
+      </c>
+      <c r="D939" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="940" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B940" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="C940" s="7">
+        <v>5.5999999999999999E-3</v>
+      </c>
+      <c r="D940" s="7">
+        <v>3.3999999999999998E-3</v>
+      </c>
+    </row>
+    <row r="941" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B941" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="C941">
+        <v>2.46E-2</v>
+      </c>
+      <c r="D941">
+        <v>1.44E-2</v>
+      </c>
+    </row>
+    <row r="943" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C943" t="s">
+        <v>81</v>
+      </c>
+      <c r="D943" t="s">
+        <v>82</v>
+      </c>
+      <c r="F943" t="s">
+        <v>81</v>
+      </c>
+      <c r="G943" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="944" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A944" s="4">
+        <v>52</v>
+      </c>
+      <c r="B944" s="3" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="945" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B945" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C945" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D945" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E945" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F945" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G945" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="946" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B946" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="C946">
+        <v>6.3E-2</v>
+      </c>
+      <c r="E946" t="s">
+        <v>274</v>
+      </c>
+      <c r="F946" s="2">
+        <v>1.407E-4</v>
+      </c>
+      <c r="G946" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="947" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B947" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C947">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="948" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B948" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C948">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="949" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B949" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C949">
+        <v>9.6</v>
+      </c>
+      <c r="D949">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="950" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B950" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="C950">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="D950">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="951" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B951" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="C951">
+        <v>0.4516</v>
+      </c>
+      <c r="D951">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="952" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B952" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C952" s="2">
+        <v>5590.2</v>
+      </c>
+    </row>
+    <row r="953" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B953" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C953">
+        <v>1.4E-3</v>
+      </c>
+      <c r="D953" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="954" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B954" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="C954" s="7">
+        <v>2.35E-2</v>
+      </c>
+      <c r="D954" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="955" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B955" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="C955" s="7">
+        <v>5.5999999999999999E-3</v>
+      </c>
+      <c r="D955" s="7">
+        <v>3.3999999999999998E-3</v>
+      </c>
+    </row>
+    <row r="956" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B956" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="C956">
+        <v>2.46E-2</v>
+      </c>
+      <c r="D956">
+        <v>1.44E-2</v>
+      </c>
+    </row>
+    <row r="958" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C958" t="s">
+        <v>81</v>
+      </c>
+      <c r="D958" t="s">
+        <v>82</v>
+      </c>
+      <c r="F958" t="s">
+        <v>81</v>
+      </c>
+      <c r="G958" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="959" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A959" s="4">
+        <v>53</v>
+      </c>
+      <c r="B959" s="3" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="960" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B960" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C960" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D960" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E960" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F960" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G960" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="961" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B961" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="C961">
+        <v>6.3E-2</v>
+      </c>
+      <c r="E961" t="s">
+        <v>275</v>
+      </c>
+      <c r="F961" s="2">
+        <v>5.5960000000000005E-4</v>
+      </c>
+      <c r="G961" s="2">
+        <v>5.8069999999999997E-4</v>
+      </c>
+    </row>
+    <row r="962" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B962" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C962">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="963" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B963" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C963">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="964" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B964" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C964">
+        <v>9.6</v>
+      </c>
+      <c r="D964">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="965" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B965" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="C965">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="D965">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="966" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B966" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="C966">
+        <v>0.4516</v>
+      </c>
+      <c r="D966">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="967" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B967" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C967" s="2">
+        <v>5590.2</v>
+      </c>
+    </row>
+    <row r="968" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B968" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="C968" s="7">
+        <v>5.5999999999999999E-3</v>
+      </c>
+      <c r="D968" s="7">
+        <v>3.3999999999999998E-3</v>
+      </c>
+    </row>
+    <row r="969" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B969" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="C969" s="7">
+        <v>2.35E-2</v>
+      </c>
+      <c r="D969" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="970" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B970" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C970">
+        <v>1.4E-3</v>
+      </c>
+      <c r="D970" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="971" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B971" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="C971">
+        <v>2.46E-2</v>
+      </c>
+      <c r="D971">
+        <v>1.44E-2</v>
+      </c>
+    </row>
+    <row r="973" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C973" t="s">
+        <v>81</v>
+      </c>
+      <c r="D973" t="s">
+        <v>82</v>
+      </c>
+      <c r="F973" t="s">
+        <v>81</v>
+      </c>
+      <c r="G973" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="974" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A974" s="4">
+        <v>54</v>
+      </c>
+      <c r="B974" s="3" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="975" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B975" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C975" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D975" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E975" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F975" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G975" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="976" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B976" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="C976">
+        <v>6.3E-2</v>
+      </c>
+      <c r="E976" t="s">
+        <v>278</v>
+      </c>
+      <c r="F976" s="2">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="G976" s="2">
+        <v>2.5000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="977" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B977" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C977">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="978" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B978" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C978">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="979" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B979" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C979">
+        <v>9.6</v>
+      </c>
+      <c r="D979">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="980" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B980" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="C980">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="D980">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="981" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B981" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="C981">
+        <v>0.4516</v>
+      </c>
+      <c r="D981">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="982" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B982" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C982" s="2">
+        <v>5590.2</v>
+      </c>
+    </row>
+    <row r="983" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B983" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="C983">
+        <v>2.46E-2</v>
+      </c>
+      <c r="D983">
+        <v>1.44E-2</v>
+      </c>
+    </row>
+    <row r="984" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B984" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="C984" s="7">
+        <v>2.35E-2</v>
+      </c>
+      <c r="D984" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="985" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B985" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C985">
+        <v>1.4E-3</v>
+      </c>
+      <c r="D985" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="986" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B986" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="C986" s="7">
+        <v>5.5999999999999999E-3</v>
+      </c>
+      <c r="D986" s="7">
+        <v>3.3999999999999998E-3</v>
+      </c>
+    </row>
+    <row r="988" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C988" t="s">
+        <v>81</v>
+      </c>
+      <c r="D988" t="s">
+        <v>82</v>
+      </c>
+      <c r="F988" t="s">
+        <v>81</v>
+      </c>
+      <c r="G988" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="989" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A989" s="4">
+        <v>55</v>
+      </c>
+      <c r="B989" s="3" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="990" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B990" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C990" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D990" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E990" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F990" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G990" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="991" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B991" t="s">
+        <v>94</v>
+      </c>
+      <c r="C991">
+        <v>0.1139</v>
+      </c>
+      <c r="D991">
+        <v>0.18640000000000001</v>
+      </c>
+      <c r="E991" t="s">
+        <v>94</v>
+      </c>
+      <c r="F991">
+        <v>0.1139</v>
+      </c>
+      <c r="G991">
+        <v>0.18640000000000001</v>
+      </c>
+    </row>
+    <row r="992" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B992" t="s">
+        <v>120</v>
+      </c>
+      <c r="C992">
+        <v>0.1139</v>
+      </c>
+      <c r="D992">
+        <v>0.18640000000000001</v>
+      </c>
+      <c r="E992" t="s">
+        <v>120</v>
+      </c>
+      <c r="F992">
+        <v>0.1139</v>
+      </c>
+      <c r="G992">
+        <v>0.18640000000000001</v>
+      </c>
+    </row>
+    <row r="993" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B993" t="s">
+        <v>146</v>
+      </c>
+      <c r="C993">
+        <v>0.1139</v>
+      </c>
+      <c r="D993">
+        <v>0.18640000000000001</v>
+      </c>
+      <c r="E993" t="s">
+        <v>146</v>
+      </c>
+      <c r="F993">
+        <v>0.1139</v>
+      </c>
+      <c r="G993">
+        <v>0.18640000000000001</v>
+      </c>
+    </row>
+    <row r="994" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B994" t="s">
+        <v>172</v>
+      </c>
+      <c r="C994">
+        <v>2.1700000000000001E-2</v>
+      </c>
+      <c r="D994">
+        <v>3.7100000000000001E-2</v>
+      </c>
+      <c r="E994" t="s">
+        <v>172</v>
+      </c>
+      <c r="F994">
+        <v>2.1700000000000001E-2</v>
+      </c>
+      <c r="G994">
+        <v>3.7100000000000001E-2</v>
+      </c>
+    </row>
+    <row r="995" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B995" t="s">
+        <v>198</v>
+      </c>
+      <c r="C995">
+        <v>2.1700000000000001E-2</v>
+      </c>
+      <c r="D995">
+        <v>3.7100000000000001E-2</v>
+      </c>
+      <c r="E995" t="s">
+        <v>198</v>
+      </c>
+      <c r="F995">
+        <v>2.1700000000000001E-2</v>
+      </c>
+      <c r="G995">
+        <v>3.7100000000000001E-2</v>
+      </c>
+    </row>
+    <row r="996" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B996" t="s">
+        <v>68</v>
+      </c>
+      <c r="C996">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="D996">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="E996" t="s">
+        <v>317</v>
+      </c>
+      <c r="F996">
+        <v>0.26840000000000003</v>
+      </c>
+      <c r="G996">
+        <v>0.2104</v>
+      </c>
+    </row>
+    <row r="997" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B997" t="s">
+        <v>69</v>
+      </c>
+      <c r="C997">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="D997">
+        <v>1.1999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="998" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B998" t="s">
+        <v>70</v>
+      </c>
+      <c r="C998">
+        <v>4.7999999999999996E-3</v>
+      </c>
+      <c r="D998">
+        <v>4.7999999999999996E-3</v>
+      </c>
+    </row>
+    <row r="999" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B999" t="s">
+        <v>71</v>
+      </c>
+      <c r="C999">
+        <v>1.9</v>
+      </c>
+      <c r="D999">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="1000" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1000" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1000">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="D1000">
+        <v>5.7000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="1001" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1001" t="s">
+        <v>316</v>
+      </c>
+      <c r="C1001">
+        <v>0.17</v>
+      </c>
+      <c r="D1001">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="1003" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C1003" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1003" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1003" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1003" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="1004" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1004" s="4">
+        <v>56</v>
+      </c>
+      <c r="B1004" s="3" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="1005" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1005" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1005" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1005" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1005" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1005" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1005" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="1006" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1006" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1006">
+        <v>0.1139</v>
+      </c>
+      <c r="D1006">
+        <v>0.18640000000000001</v>
+      </c>
+      <c r="E1006" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1006">
+        <v>0.1139</v>
+      </c>
+      <c r="G1006">
+        <v>0.18640000000000001</v>
+      </c>
+    </row>
+    <row r="1008" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C1008" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1008" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1008" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1008" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="1009" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1009" s="4">
+        <v>57</v>
+      </c>
+      <c r="B1009" s="3" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="1010" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1010" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1010" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1010" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1010" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1010" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1010" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="1011" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1011" t="s">
+        <v>120</v>
+      </c>
+      <c r="C1011">
+        <v>0.1139</v>
+      </c>
+      <c r="D1011">
+        <v>0.18640000000000001</v>
+      </c>
+      <c r="E1011" t="s">
+        <v>123</v>
+      </c>
+      <c r="F1011">
+        <v>0.1139</v>
+      </c>
+      <c r="G1011">
+        <v>0.18640000000000001</v>
+      </c>
+    </row>
+    <row r="1013" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C1013" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1013" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1013" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1013" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="1014" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1014" s="4">
+        <v>58</v>
+      </c>
+      <c r="B1014" s="3" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="1015" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1015" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1015" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1015" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1015" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1015" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1015" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="1016" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1016" t="s">
+        <v>146</v>
+      </c>
+      <c r="C1016">
+        <v>0.1139</v>
+      </c>
+      <c r="D1016">
+        <v>0.18640000000000001</v>
+      </c>
+      <c r="E1016" t="s">
+        <v>149</v>
+      </c>
+      <c r="F1016">
+        <v>0.1139</v>
+      </c>
+      <c r="G1016">
+        <v>0.18640000000000001</v>
+      </c>
+    </row>
+    <row r="1018" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C1018" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1018" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1018" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1018" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="1019" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1019" s="4">
+        <v>59</v>
+      </c>
+      <c r="B1019" s="3" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="1020" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1020" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1020" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1020" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1020" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1020" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1020" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="1021" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1021" t="s">
+        <v>172</v>
+      </c>
+      <c r="C1021">
+        <v>2.1700000000000001E-2</v>
+      </c>
+      <c r="D1021">
+        <v>3.7100000000000001E-2</v>
+      </c>
+      <c r="E1021" t="s">
+        <v>175</v>
+      </c>
+      <c r="F1021">
+        <v>2.24E-2</v>
+      </c>
+      <c r="G1021">
+        <v>3.78E-2</v>
+      </c>
+    </row>
+    <row r="1022" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1022" t="s">
+        <v>169</v>
+      </c>
+      <c r="C1022" s="2">
+        <v>5.8909999999999995E-4</v>
+      </c>
+      <c r="D1022" s="2">
+        <v>5.1829999999999997E-4</v>
+      </c>
+    </row>
+    <row r="1023" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1023" t="s">
+        <v>170</v>
+      </c>
+      <c r="C1023" s="2">
+        <v>3.2129999999999999E-5</v>
+      </c>
+      <c r="D1023" s="2">
+        <v>2.8269999999999999E-5</v>
+      </c>
+    </row>
+    <row r="1024" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1024" t="s">
+        <v>171</v>
+      </c>
+      <c r="C1024" s="2">
+        <v>1.2850000000000001E-4</v>
+      </c>
+      <c r="D1024" s="2">
+        <v>1.131E-4</v>
+      </c>
+    </row>
+    <row r="1026" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C1026" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1026" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1026" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1026" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="1027" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1027" s="4">
+        <v>60</v>
+      </c>
+      <c r="B1027" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="1028" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1028" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1028" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1028" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1028" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1028" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1028" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="1029" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1029" t="s">
+        <v>198</v>
+      </c>
+      <c r="C1029">
+        <v>2.1700000000000001E-2</v>
+      </c>
+      <c r="D1029">
+        <v>3.7100000000000001E-2</v>
+      </c>
+      <c r="E1029" t="s">
+        <v>201</v>
+      </c>
+      <c r="F1029">
+        <v>2.24E-2</v>
+      </c>
+      <c r="G1029">
+        <v>3.78E-2</v>
+      </c>
+    </row>
+    <row r="1030" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1030" t="s">
+        <v>195</v>
+      </c>
+      <c r="C1030" s="2">
+        <v>5.8909999999999995E-4</v>
+      </c>
+      <c r="D1030" s="2">
+        <v>5.1829999999999997E-4</v>
+      </c>
+    </row>
+    <row r="1031" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1031" t="s">
+        <v>196</v>
+      </c>
+      <c r="C1031" s="2">
+        <v>3.2129999999999999E-5</v>
+      </c>
+      <c r="D1031" s="2">
+        <v>2.8269999999999999E-5</v>
+      </c>
+    </row>
+    <row r="1032" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1032" t="s">
+        <v>197</v>
+      </c>
+      <c r="C1032" s="2">
+        <v>1.2850000000000001E-4</v>
+      </c>
+      <c r="D1032" s="2">
+        <v>1.131E-4</v>
+      </c>
+    </row>
+    <row r="1034" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C1034" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1034" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1034" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1034" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="1035" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1035" s="4">
+        <v>61</v>
+      </c>
+      <c r="B1035" s="3" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="1036" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1036" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1036" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1036" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1036" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1036" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1036" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="1037" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1037" t="s">
+        <v>226</v>
+      </c>
+      <c r="C1037">
+        <v>2.1399999999999999E-2</v>
+      </c>
+      <c r="D1037">
+        <v>1.29E-2</v>
+      </c>
+      <c r="E1037" t="s">
+        <v>227</v>
+      </c>
+      <c r="F1037">
+        <v>2.1399999999999999E-2</v>
+      </c>
+      <c r="G1037">
+        <v>1.29E-2</v>
+      </c>
+    </row>
+    <row r="1039" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C1039" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1039" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1039" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1039" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="1040" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1040" s="4">
+        <v>62</v>
+      </c>
+      <c r="B1040" s="3" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="1041" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1041" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1041" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1041" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1041" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1041" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1041" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="1042" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1042" t="s">
+        <v>247</v>
+      </c>
+      <c r="C1042">
+        <v>4.8999999999999998E-3</v>
+      </c>
+      <c r="D1042">
+        <v>7.4000000000000003E-3</v>
+      </c>
+      <c r="E1042" t="s">
+        <v>253</v>
+      </c>
+      <c r="F1042">
+        <v>5.1999999999999998E-3</v>
+      </c>
+      <c r="G1042">
+        <v>7.7999999999999996E-3</v>
+      </c>
+    </row>
+    <row r="1043" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1043" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1043" s="2">
+        <v>2.9530000000000002E-4</v>
+      </c>
+      <c r="D1043" s="2">
+        <v>4.4200000000000001E-4</v>
+      </c>
+    </row>
+    <row r="1044" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1044" t="s">
+        <v>249</v>
+      </c>
+      <c r="C1044">
+        <v>0</v>
+      </c>
+      <c r="D1044">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1046" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C1046" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1046" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1046" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1046" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="1047" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1047" s="4">
+        <v>63</v>
+      </c>
+      <c r="B1047" s="3" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="1048" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1048" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1048" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1048" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1048" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1048" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1048" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="1049" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1049" t="s">
+        <v>273</v>
+      </c>
+      <c r="C1049">
+        <v>2.3E-3</v>
+      </c>
+      <c r="D1049">
+        <v>0</v>
+      </c>
+      <c r="E1049" t="s">
+        <v>279</v>
+      </c>
+      <c r="F1049">
+        <v>5.4999999999999997E-3</v>
+      </c>
+      <c r="G1049">
+        <v>3.0999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="1050" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1050" t="s">
+        <v>274</v>
+      </c>
+      <c r="C1050" s="2">
+        <v>1.407E-4</v>
+      </c>
+      <c r="D1050">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1051" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1051" t="s">
+        <v>275</v>
+      </c>
+      <c r="C1051" s="2">
+        <v>5.5960000000000005E-4</v>
+      </c>
+      <c r="D1051" s="2">
+        <v>5.8069999999999997E-4</v>
+      </c>
+    </row>
+    <row r="1052" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1052" t="s">
+        <v>278</v>
+      </c>
+      <c r="C1052">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="D1052">
+        <v>2.5000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="1054" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C1054" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1054" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1054" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1054" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="1055" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1055" s="4">
+        <v>64</v>
+      </c>
+      <c r="B1055" s="3" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="1056" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1056" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1056" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1056" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1056" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1056" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1056" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="1057" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1057" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="C1057">
+        <v>6.3E-2</v>
+      </c>
+      <c r="E1057" t="s">
+        <v>106</v>
+      </c>
+      <c r="F1057">
+        <v>0.82420000000000004</v>
+      </c>
+      <c r="G1057">
+        <v>0.9012</v>
+      </c>
+    </row>
+    <row r="1058" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1058" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1058">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1059" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1059" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1059">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="1060" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1060" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C1060">
+        <v>0.1139</v>
+      </c>
+      <c r="D1060">
+        <v>0.18640000000000001</v>
+      </c>
+    </row>
+    <row r="1061" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1061" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C1061">
+        <v>9.6</v>
+      </c>
+      <c r="D1061">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1062" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1062" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="C1062">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="D1062">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="1063" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1063" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1063">
+        <v>1</v>
+      </c>
+      <c r="D1063">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1064" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1064" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1064">
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="1066" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C1066" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1066" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1066" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1066" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="1067" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1067" s="4">
+        <v>65</v>
+      </c>
+      <c r="B1067" s="3" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="1068" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1068" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1068" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1068" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1068" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1068" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1068" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="1069" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1069" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="C1069">
+        <v>6.3E-2</v>
+      </c>
+      <c r="E1069" t="s">
+        <v>132</v>
+      </c>
+      <c r="F1069">
+        <v>0.82420000000000004</v>
+      </c>
+      <c r="G1069">
+        <v>0.9012</v>
+      </c>
+    </row>
+    <row r="1070" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1070" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1070">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1071" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1071" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1071">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="1072" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1072" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C1072">
+        <v>0.1139</v>
+      </c>
+      <c r="D1072">
+        <v>0.18640000000000001</v>
+      </c>
+    </row>
+    <row r="1073" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1073" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C1073">
+        <v>9.6</v>
+      </c>
+      <c r="D1073">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1074" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1074" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="C1074">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="D1074">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="1075" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1075" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="C1075">
+        <v>1</v>
+      </c>
+      <c r="D1075">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1076" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1076" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1076">
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="1077" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1077" s="1"/>
+    </row>
+    <row r="1078" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C1078" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1078" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1078" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1078" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="1079" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1079" s="4">
+        <v>66</v>
+      </c>
+      <c r="B1079" s="3" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="1080" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1080" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1080" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1080" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1080" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1080" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1080" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="1081" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1081" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="C1081">
+        <v>6.3E-2</v>
+      </c>
+      <c r="E1081" t="s">
+        <v>158</v>
+      </c>
+      <c r="F1081">
+        <v>0.82420000000000004</v>
+      </c>
+      <c r="G1081">
+        <v>0.9012</v>
+      </c>
+    </row>
+    <row r="1082" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1082" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1082">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1083" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1083" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1083">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="1084" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1084" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C1084">
+        <v>0.1139</v>
+      </c>
+      <c r="D1084">
+        <v>0.18640000000000001</v>
+      </c>
+    </row>
+    <row r="1085" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1085" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C1085">
+        <v>9.6</v>
+      </c>
+      <c r="D1085">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1086" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1086" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="C1086">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="D1086">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="1087" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1087" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C1087">
+        <v>1</v>
+      </c>
+      <c r="D1087">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1088" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1088" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1088">
+        <v>2.24E-2</v>
+      </c>
+    </row>
+    <row r="1089" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1089" s="1"/>
+    </row>
+    <row r="1090" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C1090" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1090" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1090" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1090" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="1091" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1091" s="4">
+        <v>67</v>
+      </c>
+      <c r="B1091" s="3" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="1092" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1092" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1092" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1092" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1092" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1092" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1092" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="1093" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1093" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="C1093">
+        <v>6.3E-2</v>
+      </c>
+      <c r="E1093" t="s">
+        <v>184</v>
+      </c>
+      <c r="F1093">
+        <v>0.76790000000000003</v>
+      </c>
+      <c r="G1093">
+        <v>0.86360000000000003</v>
+      </c>
+    </row>
+    <row r="1094" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1094" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1094">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1095" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1095" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1095">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="1096" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1096" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C1096">
+        <v>0.1139</v>
+      </c>
+      <c r="D1096">
+        <v>0.18640000000000001</v>
+      </c>
+    </row>
+    <row r="1097" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1097" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C1097">
+        <v>9.6</v>
+      </c>
+      <c r="D1097">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1098" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1098" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="C1098">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="D1098">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="1099" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1099" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C1099">
+        <v>1</v>
+      </c>
+      <c r="D1099">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1100" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1100" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1100">
+        <v>11.180300000000001</v>
+      </c>
+    </row>
+    <row r="1102" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C1102" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1102" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1102" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1102" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="1103" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1103" s="4">
+        <v>68</v>
+      </c>
+      <c r="B1103" s="3" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="1104" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1104" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1104" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1104" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1104" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1104" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1104" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="1105" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1105" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="C1105">
+        <v>6.3E-2</v>
+      </c>
+      <c r="E1105" t="s">
+        <v>210</v>
+      </c>
+      <c r="F1105">
+        <v>0.76790000000000003</v>
+      </c>
+      <c r="G1105">
+        <v>0.86360000000000003</v>
+      </c>
+    </row>
+    <row r="1106" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1106" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1106">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1107" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1107" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1107">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="1108" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1108" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C1108">
+        <v>0.1139</v>
+      </c>
+      <c r="D1108">
+        <v>0.18640000000000001</v>
+      </c>
+    </row>
+    <row r="1109" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1109" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C1109">
+        <v>9.6</v>
+      </c>
+      <c r="D1109">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1110" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1110" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="C1110">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="D1110">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="1111" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1111" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C1111">
+        <v>1</v>
+      </c>
+      <c r="D1111">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1112" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1112" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1112">
+        <v>11.180300000000001</v>
+      </c>
+    </row>
+    <row r="1113" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1113" s="1"/>
+    </row>
+    <row r="1114" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C1114" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1114" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1114" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1114" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="1115" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1115" s="4">
+        <v>69</v>
+      </c>
+      <c r="B1115" s="3" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="1116" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1116" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1116" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1116" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1116" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1116" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1116" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="1117" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1117" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="C1117">
+        <v>6.3E-2</v>
+      </c>
+      <c r="E1117" t="s">
+        <v>236</v>
+      </c>
+      <c r="F1117">
+        <v>0.74680000000000002</v>
+      </c>
+      <c r="G1117">
+        <v>0.74070000000000003</v>
+      </c>
+    </row>
+    <row r="1118" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1118" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1118">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1119" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1119" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1119">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="1120" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1120" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C1120">
+        <v>0.1139</v>
+      </c>
+      <c r="D1120">
+        <v>0.18640000000000001</v>
+      </c>
+    </row>
+    <row r="1121" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1121" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C1121">
+        <v>9.6</v>
+      </c>
+      <c r="D1121">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1122" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1122" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="C1122">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="D1122">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="1123" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1123" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C1123">
+        <v>0</v>
+      </c>
+      <c r="D1123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1124" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1124" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1124">
+        <v>11.180300000000001</v>
+      </c>
+    </row>
+    <row r="1126" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C1126" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1126" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1126" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1126" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="1127" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1127" s="4">
+        <v>70</v>
+      </c>
+      <c r="B1127" s="3" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="1128" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1128" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1128" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1128" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1128" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1128" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1128" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="1129" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1129" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="C1129">
+        <v>6.3E-2</v>
+      </c>
+      <c r="E1129" t="s">
+        <v>262</v>
+      </c>
+      <c r="F1129">
+        <v>0.84440000000000004</v>
+      </c>
+      <c r="G1129">
+        <v>0.84440000000000004</v>
+      </c>
+    </row>
+    <row r="1130" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1130" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1130">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1131" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1131" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1131">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="1132" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1132" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="C1132">
+        <v>0.1139</v>
+      </c>
+      <c r="D1132">
+        <v>0.18640000000000001</v>
+      </c>
+    </row>
+    <row r="1133" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1133" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C1133">
+        <v>9.6</v>
+      </c>
+      <c r="D1133">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1134" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1134" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="C1134">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="D1134">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="1135" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1135" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C1135">
+        <v>1</v>
+      </c>
+      <c r="D1135">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1136" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1136" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1136" s="2">
+        <v>5590.2</v>
+      </c>
+    </row>
+    <row r="1137" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1137" s="1"/>
+    </row>
+    <row r="1138" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C1138" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1138" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1138" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1138" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="1139" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1139" s="4">
+        <v>71</v>
+      </c>
+      <c r="B1139" s="3" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="1140" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1140" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1140" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1140" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1140" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1140" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1140" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="1141" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1141" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="C1141">
+        <v>6.3E-2</v>
+      </c>
+      <c r="E1141" t="s">
+        <v>288</v>
+      </c>
+      <c r="F1141">
+        <v>0.90010000000000001</v>
+      </c>
+      <c r="G1141">
+        <v>0.82799999999999996</v>
+      </c>
+    </row>
+    <row r="1142" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1142" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1142">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1143" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1143" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1143">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="1144" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1144" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1144">
+        <v>0.1139</v>
+      </c>
+      <c r="D1144">
+        <v>0.18640000000000001</v>
+      </c>
+    </row>
+    <row r="1145" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1145" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C1145">
+        <v>9.6</v>
+      </c>
+      <c r="D1145">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="1146" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1146" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="C1146">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="D1146">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="1147" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1147" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="C1147">
+        <v>0.4516</v>
+      </c>
+      <c r="D1147">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1148" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1148" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1148" s="2">
+        <v>5590.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>